<commit_message>
Updated vintage calculations. Incorporated EPU and S&P data.
</commit_message>
<xml_diff>
--- a/Mean_PGDP_Level.xlsx
+++ b/Mean_PGDP_Level.xlsx
@@ -5,17 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b09e99cea646701/Bloomberg/Projects/FOMC/FOMC Paper/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b09e99cea646701/Bloomberg/Projects/FOMC/FOMC Paper/FOMC_Sentiment_Macro_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_80747DD93181FB4060BC27527EC8A3E3327AAEE5" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2EE1E167-8588-4EF8-BB9B-57AC5CC54655}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_80747DD93181FB4060BC27527EC8A3E3327AAEE5" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EEE25CCD-71C1-4C6F-9DC4-22D98384AE4E}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="13584" windowHeight="13524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15288" yWindow="84" windowWidth="14196" windowHeight="14736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean_Level" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -262,8 +262,8 @@
   <dimension ref="A1:J219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D213" sqref="D213:E219"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A127" sqref="A127:XFD127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.05" customHeight="1"/>

</xml_diff>